<commit_message>
added a risk to risk assessment doc, created an unfinished class diagram
</commit_message>
<xml_diff>
--- a/documents/Risk Assessment.xlsx
+++ b/documents/Risk Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ce540c5e85ced27/Documents/QA Academy/Tasdiq-Dewan-IMS-Project/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{A46510BA-57D7-44BC-9AE0-320698C8DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A38C8FA-22CC-4F6A-8078-00399D731447}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{A46510BA-57D7-44BC-9AE0-320698C8DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7838AB7-16FB-4062-A7F0-621CB47DF030}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E3750EE-0202-429F-A9C6-5E5F3C253925}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Description</t>
   </si>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>Control Measures</t>
+  </si>
+  <si>
+    <t>Accidentally drop IMS database while programme is running</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>IMS programme can no longer access a database for any commands</t>
+  </si>
+  <si>
+    <t>End application and recreate database</t>
+  </si>
+  <si>
+    <t>Only allow for CRUD sql statements within code, give no access to DROP keyword</t>
   </si>
 </sst>
 </file>
@@ -106,9 +127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,15 +450,16 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -461,14 +486,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+    <row r="2" spans="1:7" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>

</xml_diff>